<commit_message>
changes in api work of contract
</commit_message>
<xml_diff>
--- a/src/Components/Preview/ContractEntities.xlsx
+++ b/src/Components/Preview/ContractEntities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://srmtechnologies-my.sharepoint.com/personal/allen_frederick_srmtech_com/Documents/NexusLabs/CoE/Rainmaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guhan.neelakandan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95F318D5-8E62-4F39-ABCE-FD024FF09ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DADD088-F9F7-4875-912F-853052640D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7093E0CB-E4C4-4CF4-873F-872F92F22FE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7093E0CB-E4C4-4CF4-873F-872F92F22FE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>GROUP</t>
   </si>
@@ -110,21 +110,6 @@
     <t>New</t>
   </si>
   <si>
-    <t>Business Segment</t>
-  </si>
-  <si>
-    <t>Import Action</t>
-  </si>
-  <si>
-    <t>addModify</t>
-  </si>
-  <si>
-    <t>Template Name</t>
-  </si>
-  <si>
-    <t>Section Name</t>
-  </si>
-  <si>
     <t>Product Group</t>
   </si>
   <si>
@@ -167,9 +152,6 @@
     <t xml:space="preserve">WAC </t>
   </si>
   <si>
-    <t>$195</t>
-  </si>
-  <si>
     <t>Tier 1</t>
   </si>
   <si>
@@ -195,19 +177,17 @@
   </si>
   <si>
     <t>65483-2041-60</t>
-  </si>
-  <si>
-    <t>$425</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -263,6 +243,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,22 +578,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19A2BD8-0979-49D7-B75A-A19A06EB180F}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,12 +605,12 @@
       </c>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -637,7 +618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -645,7 +626,7 @@
         <v>39882</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -653,7 +634,7 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -661,7 +642,7 @@
         <v>46934</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -669,7 +650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -677,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -685,7 +666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -693,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -701,7 +682,7 @@
         <v>45800</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -709,7 +690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -717,7 +698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -725,7 +706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -733,12 +714,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -746,153 +727,125 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="6">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" t="s">
-        <v>53</v>
+      <c r="E27" s="6">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>